<commit_message>
dang nhap va dang xuat
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="222">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -42,9 +42,6 @@
     <t>trangthai</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -60,15 +57,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>giaovien</t>
-  </si>
-  <si>
-    <t>hocsinh</t>
-  </si>
-  <si>
-    <t>phuhuynh</t>
-  </si>
-  <si>
     <t>hoatdong</t>
   </si>
   <si>
@@ -87,18 +75,6 @@
     <t>$2y$10$KMjVDbnMwv28Rf6fFnfDluM7z01hX0tRxVgUMGh5fT6fVAzPqpram</t>
   </si>
   <si>
-    <t>asset/jpg/avatar-1.jpg</t>
-  </si>
-  <si>
-    <t>asset/jpg/avatar-2.jpg</t>
-  </si>
-  <si>
-    <t>asset/jpg/avatar-5.jpg</t>
-  </si>
-  <si>
-    <t>asset/jpg/avatar-4.jpg</t>
-  </si>
-  <si>
     <t>cmnd</t>
   </si>
   <si>
@@ -117,9 +93,6 @@
     <t>diachi</t>
   </si>
   <si>
-    <t>asset/jpg/avatar-3.jpg</t>
-  </si>
-  <si>
     <t>phuhuynh01</t>
   </si>
   <si>
@@ -694,6 +667,36 @@
   </si>
   <si>
     <t>Nhân viên tư vấn</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>assets/jpg/avatar-2.jpg</t>
+  </si>
+  <si>
+    <t>assets/jpg/avatar-1.jpg</t>
+  </si>
+  <si>
+    <t>assets/jpg/avatar-4.jpg</t>
+  </si>
+  <si>
+    <t>assetss/jpg/avatar-5.jpg</t>
+  </si>
+  <si>
+    <t>assets/jpg/avatar-3.jpg</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -1206,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1220,121 +1225,121 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>215</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>219</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>216</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>216</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1359,21 +1364,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C2">
         <v>1.25</v>
@@ -1381,10 +1386,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C3">
         <v>1.5</v>
@@ -1420,802 +1425,802 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
       <c r="A2" s="7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="7" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75">
       <c r="A6" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="7" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75">
       <c r="A14" s="7" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75">
       <c r="A15" s="7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="A16" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="7" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="7" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="7" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75">
       <c r="A23" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75">
       <c r="A24" s="7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75">
       <c r="A25" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75">
@@ -2734,31 +2739,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2766,28 +2771,28 @@
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F2" s="21">
         <v>3666959560</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2795,28 +2800,28 @@
         <v>123456789</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3" s="21">
         <v>3666959560</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2845,10 +2850,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2859,10 +2864,10 @@
         <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2870,10 +2875,10 @@
         <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2896,37 +2901,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="J1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2934,34 +2939,34 @@
         <v>12356</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>3666959560</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2969,34 +2974,34 @@
         <v>456789</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>3666959560</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3021,34 +3026,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3060,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3071,42 +3076,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do dl lich giao vien
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="223">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -697,6 +697,9 @@
   </si>
   <si>
     <t>assets/jpg/avatar-3.jpg</t>
+  </si>
+  <si>
+    <t>giaovien01</t>
   </si>
 </sst>
 </file>
@@ -1190,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1339,6 +1342,20 @@
         <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2726,9 +2743,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2737,7 +2756,7 @@
     <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2765,8 +2784,11 @@
       <c r="I1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>123456789</v>
       </c>
@@ -2794,8 +2816,11 @@
       <c r="I2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>123456789</v>
       </c>
@@ -2822,6 +2847,9 @@
       </c>
       <c r="I3" t="s">
         <v>196</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lam chat giua cac user
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DoAn_Final\database\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\source\repos\DoAn_Final\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="305">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -778,12 +778,180 @@
   </si>
   <si>
     <t>Nguyễn Kim</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy7</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy8</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy9</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy10</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy11</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy12</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy13</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy14</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy15</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy16</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy17</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy18</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy19</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy20</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy21</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy22</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy23</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy24</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy25</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy26</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy27</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy28</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy29</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy30</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy31</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy32</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy33</t>
+  </si>
+  <si>
+    <t>https://robohash.org/86deda626f2f117aa576e53065ca2ce6?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/d0d6b624e8dc1f6b9df0250b19663334?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/ddada9c5285e1c979bd082b3980e0477?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/63586ce4a8e58294f47deaad822de83c?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/0576129326ed4dc42e1d58ed04f154c8?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/9177ac6c2397371ec94d88c13f0e4f3d?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/9f972b73e7b85149628dd81056493d6a?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/73c70f65b271d90c898dae29003d2e55?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/5c0befd96d1599257f14037eb922dcde?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/09678e6f9451efc383f2c8d24eb1f90a?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/bd2e34edb2916044793e974353014db3?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/5c16d846cb718a7015503523723e46f5?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/0c11167f44066a7e02f50d9d53de3876?set=set1&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/1e67db6e97fe9ff5f723baec4a59631a?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/86b5c10f9c5df34bcd658abd050756e2?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/1eef6e135a795be09d567c4f6909a848?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/8a5526893b746f140df90d9417a39acf?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/9c371df7622ba95ccfe15ccbbb0d11b4?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://gravatar.com/avatar/9c371df7622ba95ccfe15ccbbb0d11b4?s=400&amp;d=robohash&amp;r=x</t>
+  </si>
+  <si>
+    <t>https://gravatar.com/avatar/286f68720bd9ca609bc091668ddff81d?s=400&amp;d=robohash&amp;r=x</t>
+  </si>
+  <si>
+    <t>https://gravatar.com/avatar/5a26990083f4554f6536976ca2709b31?s=400&amp;d=robohash&amp;r=x</t>
+  </si>
+  <si>
+    <t>https://robohash.org/5a26990083f4554f6536976ca2709b31?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/4177d5a68f2eaa97a8dfb453093f0b40?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/e7027447d22effb9e444998610f9058c?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/409f6ac3dcb017c0f1adb60b346657fa?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/744748595b4d21c613305d870d00fec7?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/592538b2ea1113619bd88d3f2523429a?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/e866d73c7124542a12050cc19366315e?set=set4&amp;bgset=&amp;size=400x400</t>
+  </si>
+  <si>
+    <t>https://robohash.org/7f43944096204a475da73679a31d6ec4?set=set4&amp;bgset=&amp;size=400x400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -913,7 +1081,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -974,6 +1142,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bình thường 2" xfId="6"/>
@@ -1273,18 +1444,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1391,7 +1562,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>220</v>
+        <v>276</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -1408,7 +1579,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>220</v>
+        <v>277</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -1425,11 +1596,14 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>213</v>
       </c>
@@ -1439,13 +1613,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>220</v>
+        <v>279</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>250</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>215</v>
@@ -1456,11 +1630,14 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>215</v>
       </c>
@@ -1470,11 +1647,14 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>220</v>
+        <v>281</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>215</v>
       </c>
@@ -1483,12 +1663,15 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>220</v>
+      <c r="A13" s="22" t="s">
+        <v>282</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>215</v>
       </c>
@@ -1498,11 +1681,14 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>220</v>
+        <v>283</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>215</v>
       </c>
@@ -1512,11 +1698,14 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>220</v>
+        <v>284</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>215</v>
       </c>
@@ -1526,11 +1715,14 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>220</v>
+        <v>285</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>215</v>
       </c>
@@ -1540,11 +1732,14 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>220</v>
+        <v>286</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>229</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>215</v>
       </c>
@@ -1553,12 +1748,15 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>220</v>
+      <c r="A18" s="22" t="s">
+        <v>287</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>215</v>
       </c>
@@ -1568,11 +1766,14 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>220</v>
+        <v>288</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>231</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>259</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>215</v>
       </c>
@@ -1582,11 +1783,14 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>232</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>215</v>
       </c>
@@ -1596,11 +1800,14 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>220</v>
+        <v>290</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>215</v>
       </c>
@@ -1610,11 +1817,14 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>220</v>
+        <v>291</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>215</v>
       </c>
@@ -1624,11 +1834,14 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>220</v>
+        <v>292</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>215</v>
       </c>
@@ -1638,11 +1851,14 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>215</v>
       </c>
@@ -1652,11 +1868,14 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>220</v>
+        <v>294</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>237</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>215</v>
       </c>
@@ -1666,11 +1885,14 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>215</v>
       </c>
@@ -1680,11 +1902,14 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>220</v>
+        <v>296</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>215</v>
       </c>
@@ -1694,11 +1919,14 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>220</v>
+        <v>297</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>215</v>
       </c>
@@ -1708,11 +1936,14 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>298</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>215</v>
       </c>
@@ -1722,11 +1953,14 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>220</v>
+        <v>299</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>215</v>
       </c>
@@ -1736,11 +1970,14 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>215</v>
       </c>
@@ -1750,11 +1987,14 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>220</v>
+        <v>301</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>215</v>
       </c>
@@ -1764,11 +2004,14 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>215</v>
       </c>
@@ -1777,12 +2020,15 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
-        <v>220</v>
+      <c r="A34" s="22" t="s">
+        <v>303</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>215</v>
       </c>
@@ -1792,11 +2038,14 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>215</v>
       </c>
@@ -1805,8 +2054,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A18" r:id="rId2"/>
+    <hyperlink ref="A34" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1818,10 +2072,10 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1866,23 +2120,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" customWidth="1"/>
     <col min="7" max="7" width="28" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1920,7 +2174,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="7" t="s">
         <v>248</v>
       </c>
@@ -1955,7 +2209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -1990,7 +2244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="7" t="s">
         <v>115</v>
       </c>
@@ -2025,7 +2279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="7" t="s">
         <v>116</v>
       </c>
@@ -2060,7 +2314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="7" t="s">
         <v>117</v>
       </c>
@@ -2095,7 +2349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="7" t="s">
         <v>118</v>
       </c>
@@ -2130,7 +2384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="7" t="s">
         <v>119</v>
       </c>
@@ -2165,7 +2419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6">
+    <row r="9" spans="1:11" ht="15.75">
       <c r="A9" s="7" t="s">
         <v>120</v>
       </c>
@@ -2200,7 +2454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6">
+    <row r="10" spans="1:11" ht="15.75">
       <c r="A10" s="7" t="s">
         <v>121</v>
       </c>
@@ -2235,7 +2489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6">
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>122</v>
       </c>
@@ -2270,7 +2524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6">
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="7" t="s">
         <v>123</v>
       </c>
@@ -2305,7 +2559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6">
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="7" t="s">
         <v>124</v>
       </c>
@@ -2340,7 +2594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6">
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="7" t="s">
         <v>125</v>
       </c>
@@ -2375,7 +2629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6">
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="7" t="s">
         <v>126</v>
       </c>
@@ -2410,7 +2664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6">
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="7" t="s">
         <v>127</v>
       </c>
@@ -2445,7 +2699,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.6">
+    <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="7" t="s">
         <v>128</v>
       </c>
@@ -2480,7 +2734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6">
+    <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="7" t="s">
         <v>129</v>
       </c>
@@ -2515,7 +2769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6">
+    <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="7" t="s">
         <v>130</v>
       </c>
@@ -2550,7 +2804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6">
+    <row r="20" spans="1:11" ht="15.75">
       <c r="A20" s="7" t="s">
         <v>131</v>
       </c>
@@ -2585,7 +2839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6">
+    <row r="21" spans="1:11" ht="15.75">
       <c r="A21" s="7" t="s">
         <v>132</v>
       </c>
@@ -2620,7 +2874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6">
+    <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="7" t="s">
         <v>133</v>
       </c>
@@ -2655,7 +2909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6">
+    <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="7" t="s">
         <v>134</v>
       </c>
@@ -2690,7 +2944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6">
+    <row r="24" spans="1:11" ht="15.75">
       <c r="A24" s="7" t="s">
         <v>135</v>
       </c>
@@ -2725,7 +2979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6">
+    <row r="25" spans="1:11" ht="15.75">
       <c r="A25" s="7" t="s">
         <v>136</v>
       </c>
@@ -2760,7 +3014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6">
+    <row r="26" spans="1:11" ht="15.75">
       <c r="A26" s="10"/>
       <c r="D26" s="3"/>
       <c r="E26" s="11"/>
@@ -2768,7 +3022,7 @@
       <c r="G26" s="16"/>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="1:11" ht="15.6">
+    <row r="27" spans="1:11" ht="15.75">
       <c r="A27" s="10"/>
       <c r="D27" s="3"/>
       <c r="E27" s="11"/>
@@ -2776,7 +3030,7 @@
       <c r="G27" s="16"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:11" ht="15.6">
+    <row r="28" spans="1:11" ht="15.75">
       <c r="A28" s="10"/>
       <c r="D28" s="3"/>
       <c r="E28" s="11"/>
@@ -2784,7 +3038,7 @@
       <c r="G28" s="16"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:11" ht="15.6">
+    <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="10"/>
       <c r="D29" s="3"/>
       <c r="E29" s="11"/>
@@ -2792,7 +3046,7 @@
       <c r="G29" s="16"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:11" ht="15.6">
+    <row r="30" spans="1:11" ht="15.75">
       <c r="A30" s="10"/>
       <c r="D30" s="3"/>
       <c r="E30" s="11"/>
@@ -2800,7 +3054,7 @@
       <c r="G30" s="16"/>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:11" ht="15.6">
+    <row r="31" spans="1:11" ht="15.75">
       <c r="A31" s="10"/>
       <c r="D31" s="3"/>
       <c r="E31" s="11"/>
@@ -2808,7 +3062,7 @@
       <c r="G31" s="16"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:11" ht="15.6">
+    <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="10"/>
       <c r="D32" s="3"/>
       <c r="E32" s="11"/>
@@ -2816,7 +3070,7 @@
       <c r="G32" s="16"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6">
+    <row r="33" spans="1:9" ht="15.75">
       <c r="A33" s="10"/>
       <c r="D33" s="3"/>
       <c r="E33" s="11"/>
@@ -2824,7 +3078,7 @@
       <c r="G33" s="16"/>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6">
+    <row r="34" spans="1:9" ht="15.75">
       <c r="A34" s="10"/>
       <c r="D34" s="3"/>
       <c r="E34" s="11"/>
@@ -2832,7 +3086,7 @@
       <c r="G34" s="16"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35" s="10"/>
       <c r="D35" s="3"/>
       <c r="E35" s="11"/>
@@ -2840,7 +3094,7 @@
       <c r="G35" s="16"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6">
+    <row r="36" spans="1:9" ht="15.75">
       <c r="A36" s="10"/>
       <c r="D36" s="3"/>
       <c r="E36" s="11"/>
@@ -2848,7 +3102,7 @@
       <c r="G36" s="16"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6">
+    <row r="37" spans="1:9" ht="15.75">
       <c r="A37" s="10"/>
       <c r="D37" s="3"/>
       <c r="E37" s="11"/>
@@ -2856,7 +3110,7 @@
       <c r="G37" s="16"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6">
+    <row r="38" spans="1:9" ht="15.75">
       <c r="A38" s="10"/>
       <c r="D38" s="3"/>
       <c r="E38" s="11"/>
@@ -2864,7 +3118,7 @@
       <c r="G38" s="16"/>
       <c r="I38" s="14"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="10"/>
       <c r="D39" s="3"/>
       <c r="E39" s="11"/>
@@ -2872,7 +3126,7 @@
       <c r="G39" s="16"/>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40" s="10"/>
       <c r="D40" s="3"/>
       <c r="E40" s="11"/>
@@ -2880,7 +3134,7 @@
       <c r="G40" s="16"/>
       <c r="I40" s="14"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6">
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="10"/>
       <c r="D41" s="3"/>
       <c r="E41" s="11"/>
@@ -2888,344 +3142,344 @@
       <c r="G41" s="16"/>
       <c r="I41" s="14"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="10"/>
       <c r="D42" s="3"/>
       <c r="E42" s="11"/>
       <c r="F42" s="2"/>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6">
+    <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="10"/>
       <c r="D43" s="3"/>
       <c r="E43" s="11"/>
       <c r="F43" s="2"/>
       <c r="I43" s="14"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6">
+    <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="10"/>
       <c r="D44" s="3"/>
       <c r="E44" s="11"/>
       <c r="F44" s="2"/>
       <c r="I44" s="14"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6">
+    <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="10"/>
       <c r="D45" s="3"/>
       <c r="E45" s="11"/>
       <c r="F45" s="2"/>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6">
+    <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="10"/>
       <c r="D46" s="3"/>
       <c r="E46" s="11"/>
       <c r="F46" s="2"/>
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6">
+    <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="10"/>
       <c r="D47" s="3"/>
       <c r="E47" s="11"/>
       <c r="F47" s="2"/>
       <c r="I47" s="14"/>
     </row>
-    <row r="50" spans="3:7" ht="15.6">
+    <row r="50" spans="3:7" ht="15.75">
       <c r="C50" s="18"/>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="3:7" ht="15.6">
+    <row r="51" spans="3:7" ht="15.75">
       <c r="C51" s="19"/>
       <c r="D51" s="11"/>
       <c r="E51" s="4"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="3:7" ht="15.6">
+    <row r="52" spans="3:7" ht="15.75">
       <c r="C52" s="19"/>
       <c r="D52" s="11"/>
       <c r="E52" s="4"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="3:7" ht="15.6">
+    <row r="53" spans="3:7" ht="15.75">
       <c r="C53" s="19"/>
       <c r="D53" s="11"/>
       <c r="E53" s="4"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="3:7" ht="15.6">
+    <row r="54" spans="3:7" ht="15.75">
       <c r="C54" s="19"/>
       <c r="D54" s="11"/>
       <c r="E54" s="4"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="3:7" ht="15.6">
+    <row r="55" spans="3:7" ht="15.75">
       <c r="C55" s="19"/>
       <c r="D55" s="11"/>
       <c r="E55" s="4"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="3:7" ht="15.6">
+    <row r="56" spans="3:7" ht="15.75">
       <c r="C56" s="19"/>
       <c r="D56" s="11"/>
       <c r="E56" s="4"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="3:7" ht="15.6">
+    <row r="57" spans="3:7" ht="15.75">
       <c r="C57" s="19"/>
       <c r="D57" s="11"/>
       <c r="E57" s="4"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="3:7" ht="15.6">
+    <row r="58" spans="3:7" ht="15.75">
       <c r="C58" s="19"/>
       <c r="D58" s="11"/>
       <c r="E58" s="6"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="3:7" ht="15.6">
+    <row r="59" spans="3:7" ht="15.75">
       <c r="C59" s="19"/>
       <c r="D59" s="11"/>
       <c r="E59" s="4"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="3:7" ht="15.6">
+    <row r="60" spans="3:7" ht="15.75">
       <c r="C60" s="19"/>
       <c r="D60" s="11"/>
       <c r="E60" s="4"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="3:7" ht="15.6">
+    <row r="61" spans="3:7" ht="15.75">
       <c r="C61" s="19"/>
       <c r="D61" s="11"/>
       <c r="E61" s="4"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="3:7" ht="15.6">
+    <row r="62" spans="3:7" ht="15.75">
       <c r="C62" s="19"/>
       <c r="D62" s="11"/>
       <c r="E62" s="4"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="3:7" ht="15.6">
+    <row r="63" spans="3:7" ht="15.75">
       <c r="C63" s="19"/>
       <c r="D63" s="11"/>
       <c r="E63" s="4"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="3:7" ht="15.6">
+    <row r="64" spans="3:7" ht="15.75">
       <c r="C64" s="19"/>
       <c r="D64" s="11"/>
       <c r="E64" s="4"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="3:7" ht="15.6">
+    <row r="65" spans="3:7" ht="15.75">
       <c r="C65" s="19"/>
       <c r="D65" s="11"/>
       <c r="E65" s="6"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="3:7" ht="15.6">
+    <row r="66" spans="3:7" ht="15.75">
       <c r="C66" s="19"/>
       <c r="D66" s="11"/>
       <c r="E66" s="4"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="3:7" ht="15.6">
+    <row r="67" spans="3:7" ht="15.75">
       <c r="C67" s="19"/>
       <c r="D67" s="11"/>
       <c r="E67" s="4"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="3:7" ht="15.6">
+    <row r="68" spans="3:7" ht="15.75">
       <c r="C68" s="18"/>
       <c r="D68" s="8"/>
       <c r="E68" s="4"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="3:7" ht="15.6">
+    <row r="69" spans="3:7" ht="15.75">
       <c r="C69" s="19"/>
       <c r="D69" s="11"/>
       <c r="E69" s="4"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="3:7" ht="15.6">
+    <row r="70" spans="3:7" ht="15.75">
       <c r="C70" s="19"/>
       <c r="D70" s="11"/>
       <c r="E70" s="4"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="3:7" ht="15.6">
+    <row r="71" spans="3:7" ht="15.75">
       <c r="C71" s="19"/>
       <c r="D71" s="11"/>
       <c r="E71" s="4"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="3:7" ht="15.6">
+    <row r="72" spans="3:7" ht="15.75">
       <c r="C72" s="19"/>
       <c r="D72" s="11"/>
       <c r="E72" s="4"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="3:7" ht="15.6">
+    <row r="73" spans="3:7" ht="15.75">
       <c r="C73" s="19"/>
       <c r="D73" s="11"/>
       <c r="E73" s="6"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="3:7" ht="15.6">
+    <row r="74" spans="3:7" ht="15.75">
       <c r="C74" s="19"/>
       <c r="D74" s="11"/>
       <c r="E74" s="6"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="3:7" ht="15.6">
+    <row r="75" spans="3:7" ht="15.75">
       <c r="C75" s="19"/>
       <c r="D75" s="11"/>
       <c r="E75" s="4"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="3:7" ht="15.6">
+    <row r="76" spans="3:7" ht="15.75">
       <c r="C76" s="19"/>
       <c r="D76" s="11"/>
       <c r="E76" s="4"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="3:7" ht="15.6">
+    <row r="77" spans="3:7" ht="15.75">
       <c r="C77" s="19"/>
       <c r="D77" s="11"/>
       <c r="E77" s="4"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="3:7" ht="15.6">
+    <row r="78" spans="3:7" ht="15.75">
       <c r="C78" s="19"/>
       <c r="D78" s="11"/>
       <c r="E78" s="4"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="3:7" ht="15.6">
+    <row r="79" spans="3:7" ht="15.75">
       <c r="C79" s="19"/>
       <c r="D79" s="11"/>
       <c r="E79" s="4"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="3:7" ht="15.6">
+    <row r="80" spans="3:7" ht="15.75">
       <c r="C80" s="19"/>
       <c r="D80" s="11"/>
       <c r="E80" s="4"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="3:7" ht="15.6">
+    <row r="81" spans="3:7" ht="15.75">
       <c r="C81" s="19"/>
       <c r="D81" s="11"/>
       <c r="E81" s="4"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="3:7" ht="15.6">
+    <row r="82" spans="3:7" ht="15.75">
       <c r="C82" s="19"/>
       <c r="D82" s="11"/>
       <c r="E82" s="6"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="3:7" ht="15.6">
+    <row r="83" spans="3:7" ht="15.75">
       <c r="C83" s="19"/>
       <c r="D83" s="11"/>
       <c r="E83" s="4"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="3:7" ht="15.6">
+    <row r="84" spans="3:7" ht="15.75">
       <c r="C84" s="19"/>
       <c r="D84" s="11"/>
       <c r="E84" s="6"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="3:7" ht="15.6">
+    <row r="85" spans="3:7" ht="15.75">
       <c r="C85" s="19"/>
       <c r="D85" s="11"/>
       <c r="E85" s="4"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="3:7" ht="15.6">
+    <row r="86" spans="3:7" ht="15.75">
       <c r="C86" s="19"/>
       <c r="D86" s="11"/>
       <c r="E86" s="4"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
     </row>
-    <row r="87" spans="3:7" ht="15.6">
+    <row r="87" spans="3:7" ht="15.75">
       <c r="C87" s="19"/>
       <c r="D87" s="11"/>
       <c r="E87" s="4"/>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
     </row>
-    <row r="88" spans="3:7" ht="15.6">
+    <row r="88" spans="3:7" ht="15.75">
       <c r="C88" s="19"/>
       <c r="D88" s="11"/>
       <c r="E88" s="4"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="3:7" ht="15.6">
+    <row r="89" spans="3:7" ht="15.75">
       <c r="C89" s="19"/>
       <c r="D89" s="11"/>
     </row>
-    <row r="90" spans="3:7" ht="15.6">
+    <row r="90" spans="3:7" ht="15.75">
       <c r="C90" s="19"/>
       <c r="D90" s="11"/>
     </row>
-    <row r="91" spans="3:7" ht="15.6">
+    <row r="91" spans="3:7" ht="15.75">
       <c r="C91" s="19"/>
       <c r="D91" s="11"/>
     </row>
-    <row r="92" spans="3:7" ht="15.6">
+    <row r="92" spans="3:7" ht="15.75">
       <c r="C92" s="19"/>
       <c r="D92" s="11"/>
     </row>
-    <row r="93" spans="3:7" ht="15.6">
+    <row r="93" spans="3:7" ht="15.75">
       <c r="C93" s="19"/>
       <c r="D93" s="11"/>
     </row>
-    <row r="94" spans="3:7" ht="15.6">
+    <row r="94" spans="3:7" ht="15.75">
       <c r="C94" s="19"/>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" spans="3:7" ht="15.6">
+    <row r="95" spans="3:7" ht="15.75">
       <c r="C95" s="19"/>
       <c r="D95" s="11"/>
     </row>
@@ -3269,11 +3523,11 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3389,11 +3643,11 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3440,11 +3694,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3567,9 +3821,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3617,9 +3871,9 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="37.6640625" customWidth="1"/>
+    <col min="1" max="3" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
tam duoc hoc phi
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="304">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -619,9 +619,6 @@
   </si>
   <si>
     <t>Hoạt động</t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
   <si>
     <t>Hiếu</t>
@@ -1444,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1463,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1477,7 +1474,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -1486,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -1494,7 +1491,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1503,7 +1500,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -1511,7 +1508,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -1520,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -1528,7 +1525,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -1537,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -1545,7 +1542,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1554,7 +1551,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
@@ -1562,7 +1559,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -1571,7 +1568,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -1579,7 +1576,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -1588,7 +1585,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
@@ -1596,16 +1593,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -1613,16 +1610,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -1630,16 +1627,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
@@ -1647,16 +1644,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
@@ -1664,16 +1661,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -1681,16 +1678,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
@@ -1698,16 +1695,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
@@ -1715,16 +1712,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
@@ -1732,16 +1729,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
@@ -1749,16 +1746,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>8</v>
@@ -1766,16 +1763,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
@@ -1783,16 +1780,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
@@ -1800,16 +1797,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
@@ -1817,16 +1814,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
@@ -1834,16 +1831,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>8</v>
@@ -1851,16 +1848,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
@@ -1868,16 +1865,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>8</v>
@@ -1885,16 +1882,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>8</v>
@@ -1902,16 +1899,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
@@ -1919,16 +1916,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>8</v>
@@ -1936,16 +1933,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>8</v>
@@ -1953,16 +1950,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>8</v>
@@ -1970,16 +1967,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>8</v>
@@ -1987,16 +1984,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>8</v>
@@ -2004,16 +2001,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>8</v>
@@ -2021,16 +2018,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>8</v>
@@ -2038,16 +2035,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>8</v>
@@ -2094,7 +2091,7 @@
         <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2">
         <v>1.25</v>
@@ -2176,7 +2173,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>70</v>
@@ -2185,7 +2182,7 @@
         <v>161</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>71</v>
@@ -2220,7 +2217,7 @@
         <v>162</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>24</v>
@@ -2255,7 +2252,7 @@
         <v>163</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>24</v>
@@ -2290,7 +2287,7 @@
         <v>164</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>24</v>
@@ -2325,7 +2322,7 @@
         <v>165</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>24</v>
@@ -2360,7 +2357,7 @@
         <v>166</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>24</v>
@@ -2395,7 +2392,7 @@
         <v>167</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>71</v>
@@ -2430,7 +2427,7 @@
         <v>168</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>71</v>
@@ -2465,7 +2462,7 @@
         <v>169</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>24</v>
@@ -2500,7 +2497,7 @@
         <v>170</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>24</v>
@@ -2535,7 +2532,7 @@
         <v>171</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>24</v>
@@ -2570,7 +2567,7 @@
         <v>172</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>71</v>
@@ -2605,7 +2602,7 @@
         <v>173</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>71</v>
@@ -2640,7 +2637,7 @@
         <v>174</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>24</v>
@@ -2675,7 +2672,7 @@
         <v>175</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>24</v>
@@ -2710,7 +2707,7 @@
         <v>176</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>71</v>
@@ -2745,7 +2742,7 @@
         <v>177</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>71</v>
@@ -2780,7 +2777,7 @@
         <v>178</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>71</v>
@@ -2815,7 +2812,7 @@
         <v>179</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>71</v>
@@ -2850,7 +2847,7 @@
         <v>180</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>71</v>
@@ -2885,7 +2882,7 @@
         <v>181</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>24</v>
@@ -2920,7 +2917,7 @@
         <v>182</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>71</v>
@@ -2955,7 +2952,7 @@
         <v>183</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>71</v>
@@ -2990,7 +2987,7 @@
         <v>184</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>71</v>
@@ -3567,13 +3564,13 @@
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -3605,7 +3602,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -3652,7 +3649,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3666,10 +3663,10 @@
         <v>303</v>
       </c>
       <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
         <v>205</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3677,10 +3674,10 @@
         <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3692,10 +3689,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
@@ -3747,7 +3747,7 @@
         <v>193</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -3767,8 +3767,8 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>196</v>
+      <c r="K2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3776,13 +3776,13 @@
         <v>456789</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" t="s">
         <v>71</v>
@@ -3802,8 +3802,8 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
-        <v>196</v>
+      <c r="K3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lam do phan quyen + auto them hoc phi
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="22" r:id="rId1"/>
-    <sheet name="permissions" sheetId="23" r:id="rId2"/>
-    <sheet name="role_permission" sheetId="24" r:id="rId3"/>
-    <sheet name="chuc_vu" sheetId="9" r:id="rId4"/>
-    <sheet name="users" sheetId="1" r:id="rId5"/>
-    <sheet name="hoc_sinh" sheetId="2" r:id="rId6"/>
-    <sheet name="giao_vien" sheetId="7" r:id="rId7"/>
-    <sheet name="phong_hoc" sheetId="21" r:id="rId8"/>
-    <sheet name="nhan_vien" sheetId="10" r:id="rId9"/>
-    <sheet name="level" sheetId="4" r:id="rId10"/>
-    <sheet name="loai_khoa_hoc" sheetId="5" r:id="rId11"/>
+    <sheet name="permission_group" sheetId="25" r:id="rId2"/>
+    <sheet name="permissions" sheetId="23" r:id="rId3"/>
+    <sheet name="role_permission" sheetId="24" r:id="rId4"/>
+    <sheet name="chuc_vu" sheetId="9" r:id="rId5"/>
+    <sheet name="users" sheetId="1" r:id="rId6"/>
+    <sheet name="hoc_sinh" sheetId="2" r:id="rId7"/>
+    <sheet name="giao_vien" sheetId="7" r:id="rId8"/>
+    <sheet name="phong_hoc" sheetId="21" r:id="rId9"/>
+    <sheet name="nhan_vien" sheetId="10" r:id="rId10"/>
+    <sheet name="level" sheetId="4" r:id="rId11"/>
+    <sheet name="loai_khoa_hoc" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="513">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -849,66 +850,12 @@
     <t>https://gravatar.com/avatar/5a26990083f4554f6536976ca2709b31?s=400&amp;d=robohash&amp;r=x</t>
   </si>
   <si>
-    <t>them-hoc-sinh</t>
-  </si>
-  <si>
-    <t>Thêm mới học sinh</t>
-  </si>
-  <si>
-    <t>sua-hoc-sinh</t>
-  </si>
-  <si>
-    <t>Xem danh sách học sinh</t>
-  </si>
-  <si>
-    <t>xem-ds-hoc-sinh</t>
-  </si>
-  <si>
-    <t>Cập nhật thông tin học sinh</t>
-  </si>
-  <si>
-    <t>xoa-hoc-sinh</t>
-  </si>
-  <si>
     <t>Xóa học sinh</t>
   </si>
   <si>
-    <t>xuat-hoc-sinh</t>
-  </si>
-  <si>
-    <t>Tạo file danh sách học sinh</t>
-  </si>
-  <si>
-    <t>Xem danh sách khóa học</t>
-  </si>
-  <si>
-    <t>Thêm mới khóa học</t>
-  </si>
-  <si>
-    <t>Cập nhật thông tin khóa học</t>
-  </si>
-  <si>
     <t>Xóa khóa học</t>
   </si>
   <si>
-    <t>Tạo file danh sách khóa học</t>
-  </si>
-  <si>
-    <t>xem-ds-khoa-hoc</t>
-  </si>
-  <si>
-    <t>them-khoa-hoc</t>
-  </si>
-  <si>
-    <t>sua-khoa-hoc</t>
-  </si>
-  <si>
-    <t>xoa-khoa-hoc</t>
-  </si>
-  <si>
-    <t>xuat-khoa-hoc</t>
-  </si>
-  <si>
     <t>role_id</t>
   </si>
   <si>
@@ -1066,6 +1013,567 @@
   </si>
   <si>
     <t>Minh</t>
+  </si>
+  <si>
+    <t>Truy vấn danh mục</t>
+  </si>
+  <si>
+    <t>tv_danhmuc</t>
+  </si>
+  <si>
+    <t>them_danhmuc</t>
+  </si>
+  <si>
+    <t>Thêm danh mục</t>
+  </si>
+  <si>
+    <t>sua_danhmuc</t>
+  </si>
+  <si>
+    <t>Cập nhật danh mục</t>
+  </si>
+  <si>
+    <t>xoa_danhmuc</t>
+  </si>
+  <si>
+    <t>Xóa danh mục</t>
+  </si>
+  <si>
+    <t>tv_nguoidung</t>
+  </si>
+  <si>
+    <t>them_nguoidung</t>
+  </si>
+  <si>
+    <t>sua_nguoidung</t>
+  </si>
+  <si>
+    <t>xoa_nguoidung</t>
+  </si>
+  <si>
+    <t>Truy vấn người dùng</t>
+  </si>
+  <si>
+    <t>Thêm người dùng</t>
+  </si>
+  <si>
+    <t>Cập nhật người dùng</t>
+  </si>
+  <si>
+    <t>Xóa người dùng</t>
+  </si>
+  <si>
+    <t>phanquyen_nguoidung</t>
+  </si>
+  <si>
+    <t>Phân quyền người dùng</t>
+  </si>
+  <si>
+    <t>tv_khoahoc</t>
+  </si>
+  <si>
+    <t>them_khoahoc</t>
+  </si>
+  <si>
+    <t>sua_khoahoc</t>
+  </si>
+  <si>
+    <t>xoa_khoahoc</t>
+  </si>
+  <si>
+    <t>tv_lophoc</t>
+  </si>
+  <si>
+    <t>them_lophoc</t>
+  </si>
+  <si>
+    <t>sua_lophoc</t>
+  </si>
+  <si>
+    <t>xoa_lophoc</t>
+  </si>
+  <si>
+    <t>tv_baigiang</t>
+  </si>
+  <si>
+    <t>them_baigiang</t>
+  </si>
+  <si>
+    <t>sua_baigiang</t>
+  </si>
+  <si>
+    <t>xoa_baigiang</t>
+  </si>
+  <si>
+    <t>tv_baitap</t>
+  </si>
+  <si>
+    <t>them_baitap</t>
+  </si>
+  <si>
+    <t>sua_baitap</t>
+  </si>
+  <si>
+    <t>xoa_baitap</t>
+  </si>
+  <si>
+    <t>tv_lichhoc</t>
+  </si>
+  <si>
+    <t>them_lichhoc</t>
+  </si>
+  <si>
+    <t>sua_lichhoc</t>
+  </si>
+  <si>
+    <t>xoa_lichhoc</t>
+  </si>
+  <si>
+    <t>baocao_danhthu</t>
+  </si>
+  <si>
+    <t>tv_hoccu</t>
+  </si>
+  <si>
+    <t>them_hoccu</t>
+  </si>
+  <si>
+    <t>sua_hoccu</t>
+  </si>
+  <si>
+    <t>xoa_hoccu</t>
+  </si>
+  <si>
+    <t>chia_hoccu</t>
+  </si>
+  <si>
+    <t>tv_giaovien</t>
+  </si>
+  <si>
+    <t>them_giaovien</t>
+  </si>
+  <si>
+    <t>sua_giaovien</t>
+  </si>
+  <si>
+    <t>xoa_giaovien</t>
+  </si>
+  <si>
+    <t>tv_hocsinh</t>
+  </si>
+  <si>
+    <t>them_hocsinh</t>
+  </si>
+  <si>
+    <t>sua_hocsinh</t>
+  </si>
+  <si>
+    <t>xoa_hocsinh</t>
+  </si>
+  <si>
+    <t>tv_khoanthu</t>
+  </si>
+  <si>
+    <t>them_khoanthu</t>
+  </si>
+  <si>
+    <t>sua_khoanthu</t>
+  </si>
+  <si>
+    <t>xoa_khoanthu</t>
+  </si>
+  <si>
+    <t>tv_hocphi</t>
+  </si>
+  <si>
+    <t>them_hocphi</t>
+  </si>
+  <si>
+    <t>sua_hocphi</t>
+  </si>
+  <si>
+    <t>xoa_hocphi</t>
+  </si>
+  <si>
+    <t>tv_phieuchi</t>
+  </si>
+  <si>
+    <t>them_phieuchi</t>
+  </si>
+  <si>
+    <t>sua_phieuchi</t>
+  </si>
+  <si>
+    <t>xoa_phieuchi</t>
+  </si>
+  <si>
+    <t>tv_phanlop</t>
+  </si>
+  <si>
+    <t>them_phanlop</t>
+  </si>
+  <si>
+    <t>sua_phanlop</t>
+  </si>
+  <si>
+    <t>xoa_phanlop</t>
+  </si>
+  <si>
+    <t>tv_lichhen</t>
+  </si>
+  <si>
+    <t>them_lichhen</t>
+  </si>
+  <si>
+    <t>sua_lichhen</t>
+  </si>
+  <si>
+    <t>xoa_lichhen</t>
+  </si>
+  <si>
+    <t>tv_nhanvien</t>
+  </si>
+  <si>
+    <t>them_nhanvien</t>
+  </si>
+  <si>
+    <t>sua_nhanvien</t>
+  </si>
+  <si>
+    <t>xoa_nhanvien</t>
+  </si>
+  <si>
+    <t>tv_chamconggiaovien</t>
+  </si>
+  <si>
+    <t>them_chamconggiaovien</t>
+  </si>
+  <si>
+    <t>sua_chamconggiaovien</t>
+  </si>
+  <si>
+    <t>xoa_chamconggiaovien</t>
+  </si>
+  <si>
+    <t>tv_chamcongnhanvien</t>
+  </si>
+  <si>
+    <t>them_chamcongnhanvien</t>
+  </si>
+  <si>
+    <t>sua_chamcongnhanvien</t>
+  </si>
+  <si>
+    <t>xoa_chamcongnhanvien</t>
+  </si>
+  <si>
+    <t>tv_bangchamcong</t>
+  </si>
+  <si>
+    <t>them_bangchamcong</t>
+  </si>
+  <si>
+    <t>sua_bangchamcong</t>
+  </si>
+  <si>
+    <t>xoa_bangchamcong</t>
+  </si>
+  <si>
+    <t>tv_bangluong</t>
+  </si>
+  <si>
+    <t>them_bangluong</t>
+  </si>
+  <si>
+    <t>sua_bangluong</t>
+  </si>
+  <si>
+    <t>xoa_bangluong</t>
+  </si>
+  <si>
+    <t>Truy vấn khóa học</t>
+  </si>
+  <si>
+    <t>Thêm khóa học</t>
+  </si>
+  <si>
+    <t>Cập nhật khóa học</t>
+  </si>
+  <si>
+    <t>Truy vấn bài giảng</t>
+  </si>
+  <si>
+    <t>Thêm bài giảng</t>
+  </si>
+  <si>
+    <t>Cập nhật bài giảng</t>
+  </si>
+  <si>
+    <t>Xóa bài giảng</t>
+  </si>
+  <si>
+    <t>Truy vấn bài tập</t>
+  </si>
+  <si>
+    <t>Thêm bài tập</t>
+  </si>
+  <si>
+    <t>Cập nhật bài tập</t>
+  </si>
+  <si>
+    <t>Xóa bài tập</t>
+  </si>
+  <si>
+    <t>Truy vấn lớp học</t>
+  </si>
+  <si>
+    <t>Thêm lớp học</t>
+  </si>
+  <si>
+    <t>Cập nhật lớp học</t>
+  </si>
+  <si>
+    <t>Xóa lớp học</t>
+  </si>
+  <si>
+    <t>Truy vấn lịch học</t>
+  </si>
+  <si>
+    <t>Thêm lịch học</t>
+  </si>
+  <si>
+    <t>Cập nhật lịch học</t>
+  </si>
+  <si>
+    <t>Xóa lịch học</t>
+  </si>
+  <si>
+    <t>Báo cáo danh thu</t>
+  </si>
+  <si>
+    <t>Truy vấn học cụ</t>
+  </si>
+  <si>
+    <t>Thêm học cụ</t>
+  </si>
+  <si>
+    <t>Cập nhật học cụ</t>
+  </si>
+  <si>
+    <t>Xóa học cụ</t>
+  </si>
+  <si>
+    <t>Truy vấn giáo viên</t>
+  </si>
+  <si>
+    <t>Thêm giáo viên</t>
+  </si>
+  <si>
+    <t>Cập nhật giáo viên</t>
+  </si>
+  <si>
+    <t>Xóa giáo viên</t>
+  </si>
+  <si>
+    <t>Truy vấn học sinh</t>
+  </si>
+  <si>
+    <t>Thêm học sinh</t>
+  </si>
+  <si>
+    <t>Cập nhật học sinh</t>
+  </si>
+  <si>
+    <t>Truy vấn khoản thu</t>
+  </si>
+  <si>
+    <t>Thêm khoản thu</t>
+  </si>
+  <si>
+    <t>Cập nhật khoản thu</t>
+  </si>
+  <si>
+    <t>Xóa khoản thu</t>
+  </si>
+  <si>
+    <t>Truy vấn học phí</t>
+  </si>
+  <si>
+    <t>Thêm học phí</t>
+  </si>
+  <si>
+    <t>Cập nhật học phí</t>
+  </si>
+  <si>
+    <t>Xóa học phí</t>
+  </si>
+  <si>
+    <t>Truy vấn phiếu chi</t>
+  </si>
+  <si>
+    <t>Thêm phiếu chi</t>
+  </si>
+  <si>
+    <t>Cập nhật phiếu chi</t>
+  </si>
+  <si>
+    <t>Xóa phiếu chi</t>
+  </si>
+  <si>
+    <t>Truy vấn phân lớp</t>
+  </si>
+  <si>
+    <t>Thêm phân lớp</t>
+  </si>
+  <si>
+    <t>Cập nhật phân lớp</t>
+  </si>
+  <si>
+    <t>Xóa phân lớp</t>
+  </si>
+  <si>
+    <t>Truy vấn lịch hẹn</t>
+  </si>
+  <si>
+    <t>Thêm lịch hẹn</t>
+  </si>
+  <si>
+    <t>Cập nhật lịch hẹn</t>
+  </si>
+  <si>
+    <t>Xóa lịch hẹn</t>
+  </si>
+  <si>
+    <t>Truy vấn nhân viên</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên</t>
+  </si>
+  <si>
+    <t>Cập nhật nhân viên</t>
+  </si>
+  <si>
+    <t>Xóa nhân viên</t>
+  </si>
+  <si>
+    <t>Truy vấn chấm công (giáo viên)</t>
+  </si>
+  <si>
+    <t>Thêm chấm công (giáo viên)</t>
+  </si>
+  <si>
+    <t>Cập nhật chấm công (giáo viên)</t>
+  </si>
+  <si>
+    <t>Xóa chấm công (giáo viên)</t>
+  </si>
+  <si>
+    <t>Truy vấn chấm công (nhân viên)</t>
+  </si>
+  <si>
+    <t>Thêm chấm công (nhân viên)</t>
+  </si>
+  <si>
+    <t>Cập nhật chấm công (nhân viên)</t>
+  </si>
+  <si>
+    <t>Xóa chấm công (nhân viên)</t>
+  </si>
+  <si>
+    <t>Truy vấn bảng chấm công</t>
+  </si>
+  <si>
+    <t>Thêm bảng chấm công</t>
+  </si>
+  <si>
+    <t>Cập nhật bảng chấm công</t>
+  </si>
+  <si>
+    <t>Xóa bảng chấm công</t>
+  </si>
+  <si>
+    <t>Truy vấn bảng lương</t>
+  </si>
+  <si>
+    <t>Thêm bảng lương</t>
+  </si>
+  <si>
+    <t>Cập nhật bảng lương</t>
+  </si>
+  <si>
+    <t>Xóa bảng lương</t>
+  </si>
+  <si>
+    <t>Phân chia học cụ</t>
+  </si>
+  <si>
+    <t>Tính lương</t>
+  </si>
+  <si>
+    <t>Xem bảng chấm công</t>
+  </si>
+  <si>
+    <t>Chấm công nhân viên</t>
+  </si>
+  <si>
+    <t>Chấm công giáo viên</t>
+  </si>
+  <si>
+    <t>Quản lý nhân viên</t>
+  </si>
+  <si>
+    <t>Quản lý lịch hẹn</t>
+  </si>
+  <si>
+    <t>Phân lớp</t>
+  </si>
+  <si>
+    <t>Quản lý phiếu chi</t>
+  </si>
+  <si>
+    <t>Quản lý học phí</t>
+  </si>
+  <si>
+    <t>Quản lý khoản thu</t>
+  </si>
+  <si>
+    <t>Quản lý học sinh</t>
+  </si>
+  <si>
+    <t>Quản lý giáo viên</t>
+  </si>
+  <si>
+    <t>Quản lý học cụ</t>
+  </si>
+  <si>
+    <t>Báo cáo thống kê</t>
+  </si>
+  <si>
+    <t>Điều chỉnh lịch học</t>
+  </si>
+  <si>
+    <t>Quản lý lớp học</t>
+  </si>
+  <si>
+    <t>Quản lý bài tập</t>
+  </si>
+  <si>
+    <t>Quản lý bài giảng</t>
+  </si>
+  <si>
+    <t>Quản lý khóa học</t>
+  </si>
+  <si>
+    <t>Quản lý người dùng</t>
+  </si>
+  <si>
+    <t>Quản lý danh mục</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>permission_group_id</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1716,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1275,6 +1783,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bình thường 2" xfId="6"/>
@@ -1597,7 +2106,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1605,7 +2114,7 @@
         <v>208</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1613,7 +2122,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1621,7 +2130,7 @@
         <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1630,6 +2139,175 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1677,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1737,104 +2415,192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B2" t="s">
-        <v>274</v>
+        <v>510</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B3" t="s">
-        <v>272</v>
+        <v>509</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>273</v>
-      </c>
-      <c r="B4" t="s">
-        <v>276</v>
+        <v>508</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B5" t="s">
-        <v>278</v>
+        <v>507</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" t="s">
-        <v>280</v>
+        <v>506</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" t="s">
-        <v>281</v>
+        <v>505</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8" t="s">
-        <v>282</v>
+        <v>504</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>288</v>
-      </c>
-      <c r="B9" t="s">
-        <v>283</v>
+        <v>503</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>289</v>
-      </c>
-      <c r="B10" t="s">
-        <v>284</v>
+        <v>502</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>290</v>
-      </c>
-      <c r="B11" t="s">
-        <v>285</v>
+        <v>501</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>500</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>499</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>498</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>497</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>496</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>495</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>494</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>493</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>492</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>491</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>490</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1845,10 +2611,955 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" t="s">
+        <v>333</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" t="s">
+        <v>418</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" t="s">
+        <v>419</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B13" t="s">
+        <v>420</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="s">
+        <v>421</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="s">
+        <v>422</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>354</v>
+      </c>
+      <c r="B17" t="s">
+        <v>423</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" t="s">
+        <v>425</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>357</v>
+      </c>
+      <c r="B20" t="s">
+        <v>426</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>358</v>
+      </c>
+      <c r="B21" t="s">
+        <v>427</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B22" t="s">
+        <v>428</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>349</v>
+      </c>
+      <c r="B24" t="s">
+        <v>430</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>351</v>
+      </c>
+      <c r="B26" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>360</v>
+      </c>
+      <c r="B27" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>361</v>
+      </c>
+      <c r="B28" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>362</v>
+      </c>
+      <c r="B29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>363</v>
+      </c>
+      <c r="B30" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>364</v>
+      </c>
+      <c r="B31" t="s">
+        <v>437</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>365</v>
+      </c>
+      <c r="B32" t="s">
+        <v>438</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>366</v>
+      </c>
+      <c r="B33" t="s">
+        <v>439</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>367</v>
+      </c>
+      <c r="B34" t="s">
+        <v>440</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>368</v>
+      </c>
+      <c r="B35" t="s">
+        <v>441</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>369</v>
+      </c>
+      <c r="B36" t="s">
+        <v>489</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>370</v>
+      </c>
+      <c r="B37" t="s">
+        <v>442</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>371</v>
+      </c>
+      <c r="B38" t="s">
+        <v>443</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>372</v>
+      </c>
+      <c r="B39" t="s">
+        <v>444</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>373</v>
+      </c>
+      <c r="B40" t="s">
+        <v>445</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>374</v>
+      </c>
+      <c r="B41" t="s">
+        <v>446</v>
+      </c>
+      <c r="C41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>375</v>
+      </c>
+      <c r="B42" t="s">
+        <v>447</v>
+      </c>
+      <c r="C42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>376</v>
+      </c>
+      <c r="B43" t="s">
+        <v>448</v>
+      </c>
+      <c r="C43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>377</v>
+      </c>
+      <c r="B44" t="s">
+        <v>271</v>
+      </c>
+      <c r="C44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>378</v>
+      </c>
+      <c r="B45" t="s">
+        <v>449</v>
+      </c>
+      <c r="C45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>379</v>
+      </c>
+      <c r="B46" t="s">
+        <v>450</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>380</v>
+      </c>
+      <c r="B47" t="s">
+        <v>451</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>381</v>
+      </c>
+      <c r="B48" t="s">
+        <v>452</v>
+      </c>
+      <c r="C48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>382</v>
+      </c>
+      <c r="B49" t="s">
+        <v>453</v>
+      </c>
+      <c r="C49">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>383</v>
+      </c>
+      <c r="B50" t="s">
+        <v>454</v>
+      </c>
+      <c r="C50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>384</v>
+      </c>
+      <c r="B51" t="s">
+        <v>455</v>
+      </c>
+      <c r="C51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>385</v>
+      </c>
+      <c r="B52" t="s">
+        <v>456</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>386</v>
+      </c>
+      <c r="B53" t="s">
+        <v>457</v>
+      </c>
+      <c r="C53">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>387</v>
+      </c>
+      <c r="B54" t="s">
+        <v>458</v>
+      </c>
+      <c r="C54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>388</v>
+      </c>
+      <c r="B55" t="s">
+        <v>459</v>
+      </c>
+      <c r="C55">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>389</v>
+      </c>
+      <c r="B56" t="s">
+        <v>460</v>
+      </c>
+      <c r="C56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>390</v>
+      </c>
+      <c r="B57" t="s">
+        <v>461</v>
+      </c>
+      <c r="C57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>391</v>
+      </c>
+      <c r="B58" t="s">
+        <v>462</v>
+      </c>
+      <c r="C58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>392</v>
+      </c>
+      <c r="B59" t="s">
+        <v>463</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>393</v>
+      </c>
+      <c r="B60" t="s">
+        <v>464</v>
+      </c>
+      <c r="C60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>394</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>395</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>466</v>
+      </c>
+      <c r="C62">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>396</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="C63">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>397</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="C64">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>398</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>469</v>
+      </c>
+      <c r="C65">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>399</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>470</v>
+      </c>
+      <c r="C66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>400</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>471</v>
+      </c>
+      <c r="C67">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>401</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="C68">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>473</v>
+      </c>
+      <c r="C69">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>403</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>474</v>
+      </c>
+      <c r="C70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>404</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="C71">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>405</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>476</v>
+      </c>
+      <c r="C72">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>406</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>477</v>
+      </c>
+      <c r="C73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>407</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>478</v>
+      </c>
+      <c r="C74">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>408</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>479</v>
+      </c>
+      <c r="C75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>409</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>480</v>
+      </c>
+      <c r="C76">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>410</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>481</v>
+      </c>
+      <c r="C77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>411</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C78">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>412</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>483</v>
+      </c>
+      <c r="C79">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>413</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>484</v>
+      </c>
+      <c r="C80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>414</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>485</v>
+      </c>
+      <c r="C81">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>415</v>
+      </c>
+      <c r="B82" s="24" t="s">
+        <v>486</v>
+      </c>
+      <c r="C82">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>416</v>
+      </c>
+      <c r="B83" s="24" t="s">
+        <v>487</v>
+      </c>
+      <c r="C83">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>417</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>488</v>
+      </c>
+      <c r="C84">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="B15" sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1858,10 +3569,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1949,7 +3660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1998,10 +3709,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="C4">
         <v>1.5</v>
@@ -2009,10 +3720,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="B5" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2023,11 +3734,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -2052,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -2111,7 +3822,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="23" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -2145,7 +3856,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="23" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -2162,7 +3873,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="23" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -2179,7 +3890,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="23" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>213</v>
@@ -2196,7 +3907,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="23" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>214</v>
@@ -2213,7 +3924,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="23" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>215</v>
@@ -2230,7 +3941,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="23" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>216</v>
@@ -2247,7 +3958,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="22" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>217</v>
@@ -2264,7 +3975,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="23" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>218</v>
@@ -2281,7 +3992,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="23" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>219</v>
@@ -2298,7 +4009,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="23" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>220</v>
@@ -2315,7 +4026,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="23" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>221</v>
@@ -2332,7 +4043,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="22" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>222</v>
@@ -2349,7 +4060,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="23" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>223</v>
@@ -2366,7 +4077,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="23" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>224</v>
@@ -2383,7 +4094,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="23" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>225</v>
@@ -2400,7 +4111,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="23" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>226</v>
@@ -2417,7 +4128,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="23" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>227</v>
@@ -2434,7 +4145,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="23" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>228</v>
@@ -2502,7 +4213,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="23" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>232</v>
@@ -2519,7 +4230,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="23" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>233</v>
@@ -2536,7 +4247,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="23" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>234</v>
@@ -2553,7 +4264,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="23" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>235</v>
@@ -2570,7 +4281,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="23" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>236</v>
@@ -2587,7 +4298,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="23" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>237</v>
@@ -2604,7 +4315,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>238</v>
@@ -2621,7 +4332,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>239</v>
@@ -2647,7 +4358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
@@ -4046,7 +5757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -4098,7 +5809,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="21" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
         <v>189</v>
@@ -4113,10 +5824,10 @@
         <v>22</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -4130,7 +5841,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="21" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
         <v>189</v>
@@ -4145,10 +5856,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -4169,7 +5880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4220,173 +5931,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>186</v>
-      </c>
-      <c r="J1" t="s">
-        <v>187</v>
-      </c>
-      <c r="K1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>338</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="B3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C3" t="s">
-        <v>333</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="21" t="s">
-        <v>340</v>
-      </c>
-      <c r="B4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C4" t="s">
-        <v>343</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>337</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>341</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
do dl ra dashboard tư van + dashboard admin + an bao cao thong ke
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="22" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="498">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -760,87 +760,6 @@
     <t>Nguyễn Kim</t>
   </si>
   <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy7</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy8</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy9</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy10</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy11</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy12</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy13</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy14</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy15</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy16</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy17</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy18</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy19</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy20</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy21</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy22</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy23</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy24</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy25</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy26</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy27</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy28</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy29</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy30</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy31</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy32</t>
-  </si>
-  <si>
-    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy33</t>
-  </si>
-  <si>
     <t>https://gravatar.com/avatar/9c371df7622ba95ccfe15ccbbb0d11b4?s=400&amp;d=robohash&amp;r=x</t>
   </si>
   <si>
@@ -1574,6 +1493,42 @@
   </si>
   <si>
     <t>permission_group_id</t>
+  </si>
+  <si>
+    <t>00423424</t>
+  </si>
+  <si>
+    <t>Vũ Văn</t>
+  </si>
+  <si>
+    <t>Hướng</t>
+  </si>
+  <si>
+    <t>1998/12/3</t>
+  </si>
+  <si>
+    <t>043244235</t>
+  </si>
+  <si>
+    <t>huongnv@teky.vn</t>
+  </si>
+  <si>
+    <t>https://robohash.org/7f43944096204a475da73679a31d6ec4?set=set4&amp;bgset=&amp;size=400x401</t>
+  </si>
+  <si>
+    <t>vanhanh01</t>
+  </si>
+  <si>
+    <t>03234242</t>
+  </si>
+  <si>
+    <t>1998/12/4</t>
+  </si>
+  <si>
+    <t>043244236</t>
+  </si>
+  <si>
+    <t>anhnk@teky.vn</t>
   </si>
 </sst>
 </file>
@@ -2106,7 +2061,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2114,7 +2069,7 @@
         <v>208</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2122,7 +2077,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2130,7 +2085,7 @@
         <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2140,10 +2095,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2194,7 +2149,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="21" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
         <v>189</v>
@@ -2209,7 +2164,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>320</v>
+        <v>293</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>191</v>
@@ -2229,13 +2184,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="21" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="C3" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>194</v>
@@ -2244,10 +2199,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -2264,25 +2219,25 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="21" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="B4" t="s">
         <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -2295,6 +2250,76 @@
       </c>
       <c r="K4">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="B5" t="s">
+        <v>487</v>
+      </c>
+      <c r="C5" t="s">
+        <v>488</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>491</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>192</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="B6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>496</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>497</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2302,6 +2327,8 @@
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
     <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2432,12 +2459,12 @@
         <v>204</v>
       </c>
       <c r="B1" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2445,7 +2472,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2453,7 +2480,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2461,7 +2488,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2469,7 +2496,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2477,7 +2504,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>505</v>
+        <v>478</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2485,7 +2512,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2493,7 +2520,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2501,7 +2528,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2509,7 +2536,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2517,7 +2544,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -2525,7 +2552,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2533,7 +2560,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2541,7 +2568,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2549,7 +2576,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2557,7 +2584,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2565,7 +2592,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>494</v>
+        <v>467</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2573,7 +2600,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>493</v>
+        <v>466</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -2581,7 +2608,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2589,7 +2616,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -2597,7 +2624,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2632,15 +2659,15 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2648,10 +2675,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2659,10 +2686,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2670,10 +2697,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2681,10 +2708,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2692,10 +2719,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2703,10 +2730,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2714,10 +2741,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2725,10 +2752,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="B10" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2736,10 +2763,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="B11" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2747,10 +2774,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="B12" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2758,10 +2785,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="B13" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2769,10 +2796,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="B14" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -2780,10 +2807,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="B15" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2791,10 +2818,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="B16" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2802,10 +2829,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B17" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2813,10 +2840,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
       <c r="B18" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -2824,10 +2851,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B19" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -2835,10 +2862,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="B20" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -2846,10 +2873,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
       <c r="B21" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -2857,10 +2884,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="B22" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -2868,10 +2895,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="B23" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -2879,10 +2906,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="B24" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -2890,10 +2917,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="B25" t="s">
-        <v>431</v>
+        <v>404</v>
       </c>
       <c r="C25">
         <v>6</v>
@@ -2901,10 +2928,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="B26" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -2912,10 +2939,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>360</v>
+        <v>333</v>
       </c>
       <c r="B27" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -2923,10 +2950,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="B28" t="s">
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -2934,10 +2961,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
       <c r="B29" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -2945,10 +2972,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
       <c r="B30" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -2956,10 +2983,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="B31" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -2967,10 +2994,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="B32" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="C32">
         <v>9</v>
@@ -2978,10 +3005,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="B33" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="C33">
         <v>9</v>
@@ -2989,10 +3016,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="B34" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C34">
         <v>9</v>
@@ -3000,10 +3027,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
       <c r="B35" t="s">
-        <v>441</v>
+        <v>414</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -3011,10 +3038,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>369</v>
+        <v>342</v>
       </c>
       <c r="B36" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -3022,10 +3049,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
       <c r="B37" t="s">
-        <v>442</v>
+        <v>415</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -3033,10 +3060,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="B38" t="s">
-        <v>443</v>
+        <v>416</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -3044,10 +3071,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="B39" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -3055,10 +3082,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="B40" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -3066,10 +3093,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="B41" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="C41">
         <v>11</v>
@@ -3077,10 +3104,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="B42" t="s">
-        <v>447</v>
+        <v>420</v>
       </c>
       <c r="C42">
         <v>11</v>
@@ -3088,10 +3115,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>376</v>
+        <v>349</v>
       </c>
       <c r="B43" t="s">
-        <v>448</v>
+        <v>421</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -3099,10 +3126,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="B44" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="C44">
         <v>11</v>
@@ -3110,10 +3137,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="B45" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="C45">
         <v>12</v>
@@ -3121,10 +3148,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>379</v>
+        <v>352</v>
       </c>
       <c r="B46" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="C46">
         <v>12</v>
@@ -3132,10 +3159,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="B47" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -3143,10 +3170,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="B48" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="C48">
         <v>12</v>
@@ -3154,10 +3181,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>382</v>
+        <v>355</v>
       </c>
       <c r="B49" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
       <c r="C49">
         <v>13</v>
@@ -3165,10 +3192,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>383</v>
+        <v>356</v>
       </c>
       <c r="B50" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
       <c r="C50">
         <v>13</v>
@@ -3176,10 +3203,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>384</v>
+        <v>357</v>
       </c>
       <c r="B51" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="C51">
         <v>13</v>
@@ -3187,10 +3214,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
       <c r="B52" t="s">
-        <v>456</v>
+        <v>429</v>
       </c>
       <c r="C52">
         <v>13</v>
@@ -3198,10 +3225,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>386</v>
+        <v>359</v>
       </c>
       <c r="B53" t="s">
-        <v>457</v>
+        <v>430</v>
       </c>
       <c r="C53">
         <v>14</v>
@@ -3209,10 +3236,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>387</v>
+        <v>360</v>
       </c>
       <c r="B54" t="s">
-        <v>458</v>
+        <v>431</v>
       </c>
       <c r="C54">
         <v>14</v>
@@ -3220,10 +3247,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>388</v>
+        <v>361</v>
       </c>
       <c r="B55" t="s">
-        <v>459</v>
+        <v>432</v>
       </c>
       <c r="C55">
         <v>14</v>
@@ -3231,10 +3258,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>389</v>
+        <v>362</v>
       </c>
       <c r="B56" t="s">
-        <v>460</v>
+        <v>433</v>
       </c>
       <c r="C56">
         <v>14</v>
@@ -3242,10 +3269,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>390</v>
+        <v>363</v>
       </c>
       <c r="B57" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
       <c r="C57">
         <v>15</v>
@@ -3253,10 +3280,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>391</v>
+        <v>364</v>
       </c>
       <c r="B58" t="s">
-        <v>462</v>
+        <v>435</v>
       </c>
       <c r="C58">
         <v>15</v>
@@ -3264,10 +3291,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="B59" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="C59">
         <v>15</v>
@@ -3275,10 +3302,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="B60" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
       <c r="C60">
         <v>15</v>
@@ -3286,10 +3313,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>465</v>
+        <v>438</v>
       </c>
       <c r="C61">
         <v>16</v>
@@ -3297,10 +3324,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>466</v>
+        <v>439</v>
       </c>
       <c r="C62">
         <v>16</v>
@@ -3308,10 +3335,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>467</v>
+        <v>440</v>
       </c>
       <c r="C63">
         <v>16</v>
@@ -3319,10 +3346,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>468</v>
+        <v>441</v>
       </c>
       <c r="C64">
         <v>16</v>
@@ -3330,10 +3357,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="C65">
         <v>17</v>
@@ -3341,10 +3368,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>470</v>
+        <v>443</v>
       </c>
       <c r="C66">
         <v>17</v>
@@ -3352,10 +3379,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
       <c r="C67">
         <v>17</v>
@@ -3363,10 +3390,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>472</v>
+        <v>445</v>
       </c>
       <c r="C68">
         <v>17</v>
@@ -3374,10 +3401,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>402</v>
+        <v>375</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>473</v>
+        <v>446</v>
       </c>
       <c r="C69">
         <v>18</v>
@@ -3385,10 +3412,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>403</v>
+        <v>376</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="C70">
         <v>18</v>
@@ -3396,10 +3423,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>404</v>
+        <v>377</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>475</v>
+        <v>448</v>
       </c>
       <c r="C71">
         <v>18</v>
@@ -3407,10 +3434,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>476</v>
+        <v>449</v>
       </c>
       <c r="C72">
         <v>18</v>
@@ -3418,10 +3445,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>477</v>
+        <v>450</v>
       </c>
       <c r="C73">
         <v>19</v>
@@ -3429,10 +3456,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>478</v>
+        <v>451</v>
       </c>
       <c r="C74">
         <v>19</v>
@@ -3440,10 +3467,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>479</v>
+        <v>452</v>
       </c>
       <c r="C75">
         <v>19</v>
@@ -3451,10 +3478,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>480</v>
+        <v>453</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -3462,10 +3489,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="C77">
         <v>20</v>
@@ -3473,10 +3500,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>482</v>
+        <v>455</v>
       </c>
       <c r="C78">
         <v>20</v>
@@ -3484,10 +3511,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>483</v>
+        <v>456</v>
       </c>
       <c r="C79">
         <v>20</v>
@@ -3495,10 +3522,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="C80">
         <v>20</v>
@@ -3506,10 +3533,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="C81">
         <v>21</v>
@@ -3517,10 +3544,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>415</v>
+        <v>388</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="C82">
         <v>21</v>
@@ -3528,10 +3555,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="C83">
         <v>21</v>
@@ -3539,10 +3566,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>417</v>
+        <v>390</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="C84">
         <v>21</v>
@@ -3570,10 +3597,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5190,10 +5217,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="C4">
         <v>1.5</v>
@@ -5201,10 +5228,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -5217,17 +5244,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="57.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
@@ -5244,7 +5271,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -5303,7 +5330,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="23" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -5337,7 +5364,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="23" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -5354,7 +5381,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="23" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -5371,13 +5398,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="23" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>241</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
@@ -5388,13 +5415,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="23" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>214</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -5405,13 +5432,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="23" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>215</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>243</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -5422,13 +5449,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="23" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>244</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -5439,13 +5466,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="22" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>245</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -5456,13 +5483,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="23" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>218</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -5473,13 +5500,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="23" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>247</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
@@ -5490,13 +5517,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="23" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>248</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -5507,13 +5534,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="23" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>249</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
@@ -5524,13 +5551,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="22" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>250</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -5541,13 +5568,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="23" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>223</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>251</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -5558,13 +5585,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="23" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>252</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -5575,13 +5602,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="23" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -5592,13 +5619,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="23" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>226</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>254</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -5609,13 +5636,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="23" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>227</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>255</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -5626,13 +5653,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="23" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>228</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>256</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -5643,13 +5670,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="23" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>229</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>257</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -5660,13 +5687,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="23" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>230</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
@@ -5677,13 +5704,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="23" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>231</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>259</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
@@ -5694,13 +5721,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="23" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>260</v>
+        <v>19</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -5711,13 +5738,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="23" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>233</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>261</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
@@ -5728,13 +5755,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="23" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>262</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -5745,13 +5772,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="23" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>235</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
@@ -5762,13 +5789,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="23" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>236</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
@@ -5779,13 +5806,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="23" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>237</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>265</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1">
         <v>2</v>
@@ -5796,13 +5823,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>238</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>266</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -5813,18 +5840,35 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>267</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>192</v>
       </c>
     </row>
@@ -7242,7 +7286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -7290,7 +7334,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="21" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
         <v>189</v>
@@ -7305,10 +7349,10 @@
         <v>22</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -7322,7 +7366,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="21" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>189</v>
@@ -7337,10 +7381,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
them hoc sinh bang import file
</commit_message>
<xml_diff>
--- a/database/seeders/_danh_muc_seeder.xlsx
+++ b/database/seeders/_danh_muc_seeder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DoAn_Final\database\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\source\repos\DoAn_Final\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8184"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="hoc_sinh" sheetId="2" r:id="rId1"/>
@@ -1080,7 +1080,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -1565,23 +1565,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="2" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1619,7 +1619,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>176</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="6" t="s">
         <v>98</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="6" t="s">
         <v>100</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="6" t="s">
         <v>101</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="6" t="s">
         <v>102</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="6" t="s">
         <v>103</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6">
+    <row r="9" spans="1:11" ht="15.75">
       <c r="A9" s="6" t="s">
         <v>104</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6">
+    <row r="10" spans="1:11" ht="15.75">
       <c r="A10" s="6" t="s">
         <v>105</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6">
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="6" t="s">
         <v>106</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6">
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="6" t="s">
         <v>107</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6">
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="6" t="s">
         <v>108</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6">
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="6" t="s">
         <v>109</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6">
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="6" t="s">
         <v>110</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6">
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="6" t="s">
         <v>111</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.6">
+    <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="6" t="s">
         <v>112</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6">
+    <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="6" t="s">
         <v>113</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6">
+    <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="6" t="s">
         <v>114</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6">
+    <row r="20" spans="1:11" ht="15.75">
       <c r="A20" s="6" t="s">
         <v>115</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6">
+    <row r="21" spans="1:11" ht="15.75">
       <c r="A21" s="6" t="s">
         <v>116</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6">
+    <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="6" t="s">
         <v>117</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6">
+    <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="6" t="s">
         <v>118</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6">
+    <row r="24" spans="1:11" ht="15.75">
       <c r="A24" s="6" t="s">
         <v>119</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6">
+    <row r="25" spans="1:11" ht="15.75">
       <c r="A25" s="6" t="s">
         <v>120</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6">
+    <row r="26" spans="1:11" ht="15.75">
       <c r="A26" s="9" t="s">
         <v>184</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.6">
+    <row r="27" spans="1:11" ht="15.75">
       <c r="A27" s="9" t="s">
         <v>188</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6">
+    <row r="28" spans="1:11" ht="15.75">
       <c r="A28" s="9" t="s">
         <v>193</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.6">
+    <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="9" t="s">
         <v>197</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.6">
+    <row r="30" spans="1:11" ht="15.75">
       <c r="A30" s="9" t="s">
         <v>202</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.6">
+    <row r="31" spans="1:11" ht="15.75">
       <c r="A31" s="9" t="s">
         <v>207</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.6">
+    <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="9" t="s">
         <v>211</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.6">
+    <row r="33" spans="1:11" ht="15.75">
       <c r="A33" s="9" t="s">
         <v>215</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.6">
+    <row r="34" spans="1:11" ht="15.75">
       <c r="A34" s="9" t="s">
         <v>220</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6">
+    <row r="35" spans="1:11" ht="15.75">
       <c r="A35" s="9" t="s">
         <v>225</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.6">
+    <row r="36" spans="1:11" ht="15.75">
       <c r="A36" s="9" t="s">
         <v>230</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.6">
+    <row r="37" spans="1:11" ht="15.75">
       <c r="A37" s="9" t="s">
         <v>235</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.6">
+    <row r="38" spans="1:11" ht="15.75">
       <c r="A38" s="9" t="s">
         <v>240</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.6">
+    <row r="39" spans="1:11" ht="15.75">
       <c r="A39" s="9" t="s">
         <v>244</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6">
+    <row r="40" spans="1:11" ht="15.75">
       <c r="A40" s="9" t="s">
         <v>249</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.6">
+    <row r="41" spans="1:11" ht="15.75">
       <c r="A41" s="9" t="s">
         <v>254</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6">
+    <row r="42" spans="1:11" ht="15.75">
       <c r="A42" s="9" t="s">
         <v>258</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.6">
+    <row r="43" spans="1:11" ht="15.75">
       <c r="A43" s="9" t="s">
         <v>263</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.6">
+    <row r="44" spans="1:11" ht="15.75">
       <c r="A44" s="9" t="s">
         <v>267</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.6">
+    <row r="45" spans="1:11" ht="15.75">
       <c r="A45" s="9" t="s">
         <v>271</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.6">
+    <row r="46" spans="1:11" ht="15.75">
       <c r="A46" s="9" t="s">
         <v>275</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.6">
+    <row r="47" spans="1:11" ht="15.75">
       <c r="A47" s="9" t="s">
         <v>279</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.6">
+    <row r="48" spans="1:11" ht="15.75">
       <c r="A48" s="1" t="s">
         <v>283</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.6">
+    <row r="49" spans="1:11" ht="15.75">
       <c r="A49" s="1" t="s">
         <v>288</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.6">
+    <row r="50" spans="1:11" ht="15.75">
       <c r="A50" s="1" t="s">
         <v>293</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.6">
+    <row r="51" spans="1:11" ht="15.75">
       <c r="A51" s="1" t="s">
         <v>298</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.6">
+    <row r="52" spans="1:11" ht="15.75">
       <c r="A52" s="1" t="s">
         <v>303</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6">
+    <row r="53" spans="1:11" ht="15.75">
       <c r="A53" s="1" t="s">
         <v>308</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6">
+    <row r="54" spans="1:11" ht="15.75">
       <c r="A54" s="1" t="s">
         <v>312</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.6">
+    <row r="55" spans="1:11" ht="15.75">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6">
+    <row r="56" spans="1:11" ht="15.75">
       <c r="A56" s="1" t="s">
         <v>321</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.6">
+    <row r="57" spans="1:11" ht="15.75">
       <c r="A57" s="1" t="s">
         <v>326</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.6">
+    <row r="58" spans="1:11" ht="15.75">
       <c r="A58" s="1" t="s">
         <v>330</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6">
+    <row r="59" spans="1:11" ht="15.75">
       <c r="A59" s="1" t="s">
         <v>335</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.6">
+    <row r="60" spans="1:11" ht="15.75">
       <c r="A60" s="1" t="s">
         <v>193</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6">
+    <row r="61" spans="1:11" ht="15.75">
       <c r="A61" s="1" t="s">
         <v>344</v>
       </c>
@@ -3719,219 +3719,219 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6">
+    <row r="62" spans="1:11" ht="15.75">
       <c r="C62" s="18"/>
       <c r="D62" s="10"/>
       <c r="E62" s="3"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:11" ht="15.6">
+    <row r="63" spans="1:11" ht="15.75">
       <c r="C63" s="18"/>
       <c r="D63" s="10"/>
       <c r="E63" s="3"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:11" ht="15.6">
+    <row r="64" spans="1:11" ht="15.75">
       <c r="C64" s="18"/>
       <c r="D64" s="10"/>
       <c r="E64" s="3"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="3:7" ht="15.6">
+    <row r="65" spans="3:7" ht="15.75">
       <c r="C65" s="18"/>
       <c r="D65" s="10"/>
       <c r="E65" s="5"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="3:7" ht="15.6">
+    <row r="66" spans="3:7" ht="15.75">
       <c r="C66" s="18"/>
       <c r="D66" s="10"/>
       <c r="E66" s="3"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="3:7" ht="15.6">
+    <row r="67" spans="3:7" ht="15.75">
       <c r="C67" s="18"/>
       <c r="D67" s="10"/>
       <c r="E67" s="3"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="3:7" ht="15.6">
+    <row r="68" spans="3:7" ht="15.75">
       <c r="C68" s="17"/>
       <c r="D68" s="7"/>
       <c r="E68" s="3"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="3:7" ht="15.6">
+    <row r="69" spans="3:7" ht="15.75">
       <c r="C69" s="18"/>
       <c r="D69" s="10"/>
       <c r="E69" s="3"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="3:7" ht="15.6">
+    <row r="70" spans="3:7" ht="15.75">
       <c r="C70" s="18"/>
       <c r="D70" s="10"/>
       <c r="E70" s="3"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="3:7" ht="15.6">
+    <row r="71" spans="3:7" ht="15.75">
       <c r="C71" s="18"/>
       <c r="D71" s="10"/>
       <c r="E71" s="3"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="3:7" ht="15.6">
+    <row r="72" spans="3:7" ht="15.75">
       <c r="C72" s="18"/>
       <c r="D72" s="10"/>
       <c r="E72" s="3"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="3:7" ht="15.6">
+    <row r="73" spans="3:7" ht="15.75">
       <c r="C73" s="18"/>
       <c r="D73" s="10"/>
       <c r="E73" s="5"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="3:7" ht="15.6">
+    <row r="74" spans="3:7" ht="15.75">
       <c r="C74" s="18"/>
       <c r="D74" s="10"/>
       <c r="E74" s="5"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="3:7" ht="15.6">
+    <row r="75" spans="3:7" ht="15.75">
       <c r="C75" s="18"/>
       <c r="D75" s="10"/>
       <c r="E75" s="3"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="3:7" ht="15.6">
+    <row r="76" spans="3:7" ht="15.75">
       <c r="C76" s="18"/>
       <c r="D76" s="10"/>
       <c r="E76" s="3"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="3:7" ht="15.6">
+    <row r="77" spans="3:7" ht="15.75">
       <c r="C77" s="18"/>
       <c r="D77" s="10"/>
       <c r="E77" s="3"/>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="3:7" ht="15.6">
+    <row r="78" spans="3:7" ht="15.75">
       <c r="C78" s="18"/>
       <c r="D78" s="10"/>
       <c r="E78" s="3"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="3:7" ht="15.6">
+    <row r="79" spans="3:7" ht="15.75">
       <c r="C79" s="18"/>
       <c r="D79" s="10"/>
       <c r="E79" s="3"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="3:7" ht="15.6">
+    <row r="80" spans="3:7" ht="15.75">
       <c r="C80" s="18"/>
       <c r="D80" s="10"/>
       <c r="E80" s="3"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="3:7" ht="15.6">
+    <row r="81" spans="3:7" ht="15.75">
       <c r="C81" s="18"/>
       <c r="D81" s="10"/>
       <c r="E81" s="3"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="3:7" ht="15.6">
+    <row r="82" spans="3:7" ht="15.75">
       <c r="C82" s="18"/>
       <c r="D82" s="10"/>
       <c r="E82" s="5"/>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="3:7" ht="15.6">
+    <row r="83" spans="3:7" ht="15.75">
       <c r="C83" s="18"/>
       <c r="D83" s="10"/>
       <c r="E83" s="3"/>
       <c r="F83" s="8"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="3:7" ht="15.6">
+    <row r="84" spans="3:7" ht="15.75">
       <c r="C84" s="18"/>
       <c r="D84" s="10"/>
       <c r="E84" s="5"/>
       <c r="F84" s="8"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="3:7" ht="15.6">
+    <row r="85" spans="3:7" ht="15.75">
       <c r="C85" s="18"/>
       <c r="D85" s="10"/>
       <c r="E85" s="3"/>
       <c r="F85" s="8"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="3:7" ht="15.6">
+    <row r="86" spans="3:7" ht="15.75">
       <c r="C86" s="18"/>
       <c r="D86" s="10"/>
       <c r="E86" s="3"/>
       <c r="F86" s="8"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="3:7" ht="15.6">
+    <row r="87" spans="3:7" ht="15.75">
       <c r="C87" s="18"/>
       <c r="D87" s="10"/>
       <c r="E87" s="3"/>
       <c r="F87" s="8"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="3:7" ht="15.6">
+    <row r="88" spans="3:7" ht="15.75">
       <c r="C88" s="18"/>
       <c r="D88" s="10"/>
       <c r="E88" s="3"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="3:7" ht="15.6">
+    <row r="89" spans="3:7" ht="15.75">
       <c r="C89" s="18"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="3:7" ht="15.6">
+    <row r="90" spans="3:7" ht="15.75">
       <c r="C90" s="18"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="3:7" ht="15.6">
+    <row r="91" spans="3:7" ht="15.75">
       <c r="C91" s="18"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="3:7" ht="15.6">
+    <row r="92" spans="3:7" ht="15.75">
       <c r="C92" s="18"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="3:7" ht="15.6">
+    <row r="93" spans="3:7" ht="15.75">
       <c r="C93" s="18"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="3:7" ht="15.6">
+    <row r="94" spans="3:7" ht="15.75">
       <c r="C94" s="18"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="3:7" ht="15.6">
+    <row r="95" spans="3:7" ht="15.75">
       <c r="C95" s="18"/>
       <c r="D95" s="10"/>
     </row>
@@ -3976,9 +3976,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4038,11 +4038,11 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4089,9 +4089,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4139,9 +4139,9 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="37.6640625" customWidth="1"/>
+    <col min="1" max="3" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>